<commit_message>
MAJ - articles à lire et doc
</commit_message>
<xml_diff>
--- a/drafts/Revue_litterature_catalogue.xlsx
+++ b/drafts/Revue_litterature_catalogue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33616\Desktop\MemoireDeRechercheMaster2\drafts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{09E8FDCC-DB33-49B3-918D-08B5A27E34E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558F72A0-7E8B-4E58-8049-0056082A387B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{44B06960-26D5-4330-BA7F-E7DC7C3ADA59}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="287" xr2:uid="{44B06960-26D5-4330-BA7F-E7DC7C3ADA59}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,13 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
-  <si>
-    <t>Auteur</t>
-  </si>
-  <si>
-    <t>Date de publication</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Référence complète</t>
   </si>
@@ -69,9 +63,6 @@
   </si>
   <si>
     <t>Titre</t>
-  </si>
-  <si>
-    <t>Date de lecture</t>
   </si>
   <si>
     <t>Le marketing relationnel</t>
@@ -95,22 +86,10 @@
 VOLLE Pierre</t>
   </si>
   <si>
-    <t xml:space="preserve">Théorie de la motivation intrinsèque / extrinsèque </t>
-  </si>
-  <si>
     <t>Deci
 Ryan</t>
   </si>
   <si>
-    <t xml:space="preserve">Travaux sur les leaders d'opinion </t>
-  </si>
-  <si>
-    <t>Vernette</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Management de la fidélisation : De la stratégie aux technologies digitales </t>
-  </si>
-  <si>
     <t>MEYER-WAARDEN Lars</t>
   </si>
   <si>
@@ -125,6 +104,70 @@
   <si>
     <t>MALAVAL Philippe, 
 BENAROYA Christophe</t>
+  </si>
+  <si>
+    <t>Eric Vernette
+Laurent Flores</t>
+  </si>
+  <si>
+    <t>Communiquer avec les leaders d'opinion en marketing : 
+Comment et dans quels médias ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Théorie de la motivation 
+intrinsèque / extrinsèque </t>
+  </si>
+  <si>
+    <t>Date de 
+publication</t>
+  </si>
+  <si>
+    <t>Date de 
+lecture</t>
+  </si>
+  <si>
+    <t>Auteur(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Management de la fidélisation : 
+De la stratégie aux 
+technologies digitales </t>
+  </si>
+  <si>
+    <t>Se servir de l'encadré 3 à la page 26 
+pour réfléchir au questionnaire</t>
+  </si>
+  <si>
+    <t>_ consommateur moteur
+_objectif : marketing viral
+_ utiliser l'influence du leader dans son cercle plus ou moins on line pour gagner en popularité
+_ intérêt pour le marketing d'utiliser un leader média
+_ étape 1 : communiquer avec un leader d'opinion
+une démutiplication d'audience
+une force de persuasion supérieure
+_ étape 2 : idenfier et cibler les leaders
+choix d'une méthode d'identification des leaders
+fixation d'un seuil de sélection
+_ étape 3 : cibler la communication
+choisir sa cible pour la communciation
+décrire ses attitudes et valeurs, ses caractéristiques, socio-démographiques, et comportementales
+connaître ses critères de choix
+_ étape 4 : bâtir le plan média
+choisir les médias et supports (affinitité, couverture utile , coût au mille utilie)</t>
+  </si>
+  <si>
+    <t>Il existe des leaders sur peu de catégories de produits (beauté, alimentation, voyages, mode …)</t>
+  </si>
+  <si>
+    <t>La Qualité de la relation entre la marque et le consommateur influence sur le degré de fidélité de ce dernier vis-à-vis des produits de la marque.
+Les entreprises doivent faire attention comment elle se servent des réseaux sociaux et plus particulièrement de Facebook : Facebook peut être perçu par le consommateur comme un média de communication si la marque ne met en avant que ses produits et ne cherchent pas à créer une relation avec des échanges.</t>
+  </si>
+  <si>
+    <t>Motivation : est la raison pour laquelle nous commettons des actions, peu importe lesquelles.
+Motivation intrinsèque : Relation directe entre l’individu et la tâche qu’il accomplit. Il n’y a pas de facteur externe ou de raison ultérieure de réaliser la tâche. 
+Exemple de tâche qui est une motivation intrinsèque : loisirs
+Motivation extrinsèque : La tâche réalisée est reliée à l’environnement immédiat ou à un environnement extérieur à l’exercice en cours.
+Exemple : un étudiant qui travaille pour obtenir de bonnes notes. Un employé qui fait des heures supplémentaires pour obtenir une promotion.</t>
   </si>
 </sst>
 </file>
@@ -185,11 +228,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -207,12 +253,253 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Iskoola Pota"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Iskoola Pota"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Iskoola Pota"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Iskoola Pota"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Iskoola Pota"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Iskoola Pota"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Iskoola Pota"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Iskoola Pota"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Iskoola Pota"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Iskoola Pota"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Iskoola Pota"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Iskoola Pota"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -223,6 +510,27 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{80BF0CE8-D5F6-46A6-9F43-DF34DD567FC0}" name="Tableau1" displayName="Tableau1" ref="A1:L9" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:L9" xr:uid="{532C0B04-AAD6-4E17-8F20-94CF1835A95F}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{26C2AF30-76D0-428D-8C1F-658FF5C75077}" name="Titre"/>
+    <tableColumn id="2" xr3:uid="{28BC384A-82AE-4718-A523-A36423CD26C3}" name="Date de _x000a_lecture" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{817F9A35-3879-415E-9E47-078836D9AC02}" name="Auteur(s)"/>
+    <tableColumn id="4" xr3:uid="{C79F9A3A-C10A-4950-A915-A19844A4B414}" name="Date de _x000a_publication" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{707986A3-417C-44AC-A82D-19023C1EC7AA}" name="Référence complète" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{C5A41D43-C8D9-40B7-A1C7-0B3037594B39}" name="Discipline et sous discipline" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{1D08D2D3-F62D-4D22-BBA0-B3CEC035395C}" name="Question de recherche" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{D903990C-BF65-4A47-97EE-90B85E7718C5}" name="Thèses avancées" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{FF8C8FE6-CB6A-4EA1-BDA7-953AFE517F4E}" name="Méthode" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{45A8D9EF-10D6-40F4-B531-EE9B1DCA893A}" name="Matériau empirique analysé" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{40F22F77-99BA-465D-8DB2-7E33BFAAF715}" name="Citations à utiliser" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{D4B3DD4F-9F08-4AEC-84C3-49486AF35668}" name="Remarques personnelles" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -525,130 +833,160 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="62.9453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.83984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.26171875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.3125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.3671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.83984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.26171875" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.89453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.41796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.9453125" style="3"/>
+    <col min="1" max="1" width="28.83984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5234375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.83984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7890625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.41796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="79.68359375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7890625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.26171875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="30.68359375" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.41796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.3125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.83984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.9453125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="30.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="91.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="30.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>15</v>
+      <c r="F2" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="45.9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="A3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:12" ht="61.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="153" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="275.39999999999998" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="10">
+        <v>43923</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="9">
+        <v>2004</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="45.9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="30.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>27</v>
+      <c r="A8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>26</v>
+      <c r="A9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>